<commit_message>
Create booking price and update generate
</commit_message>
<xml_diff>
--- a/src/main/resources/input_excel_file/ApiMaster.xlsx
+++ b/src/main/resources/input_excel_file/ApiMaster.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="44">
   <si>
     <t>module</t>
   </si>
@@ -56,7 +56,7 @@
     <t>test_method_name</t>
   </si>
   <si>
-    <t>login/functional</t>
+    <t>login.functional</t>
   </si>
   <si>
     <t>LoginTest</t>
@@ -80,7 +80,10 @@
     <t>login_request_template.json</t>
   </si>
   <si>
-    <t>booking/functional</t>
+    <t>testLogin</t>
+  </si>
+  <si>
+    <t>booking.functional</t>
   </si>
   <si>
     <t>QuoteFeeTest</t>
@@ -98,25 +101,31 @@
     <t>quote_fee_request_template.json</t>
   </si>
   <si>
+    <t>testQuoteFee</t>
+  </si>
+  <si>
     <t>CreateBookingBatchTest</t>
   </si>
   <si>
-    <t>bookingBatchData</t>
+    <t>createBookingBatchData</t>
   </si>
   <si>
     <t>/golf-cms/api/booking/batch</t>
   </si>
   <si>
-    <t>CreateBookingBatch.xlsx</t>
+    <t>Create_Booking_Batch.xlsx</t>
   </si>
   <si>
     <t>create_booking_batch_template.json</t>
   </si>
   <si>
-    <t>GetBookingListSelect</t>
-  </si>
-  <si>
-    <t>getBookingData</t>
+    <t>testCreateBookingBatch</t>
+  </si>
+  <si>
+    <t>GetBookingListSelectTest</t>
+  </si>
+  <si>
+    <t>getBookingListSelectData</t>
   </si>
   <si>
     <t>/golf-cms/api/booking/list/select</t>
@@ -128,13 +137,28 @@
     <t>QUERY_PARAM</t>
   </si>
   <si>
-    <t>GetBookingList.xlsx</t>
+    <t>Get_Booking_List_Select.xlsx</t>
   </si>
   <si>
     <t>(để trống)</t>
   </si>
   <si>
-    <t>GetBookingListSelectTest</t>
+    <t>testGetBookingListSelect</t>
+  </si>
+  <si>
+    <t>GetBookingPriceTest</t>
+  </si>
+  <si>
+    <t>getBookingPriceData</t>
+  </si>
+  <si>
+    <t>/golf-cms/api/booking/booking-price</t>
+  </si>
+  <si>
+    <t>booking/Get_Booking_Price.xlsx</t>
+  </si>
+  <si>
+    <t>testGetBookingPrice</t>
   </si>
 </sst>
 </file>
@@ -1352,14 +1376,14 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="5"/>
   <cols>
     <col min="1" max="1" width="24.7142857142857" customWidth="1"/>
     <col min="2" max="2" width="30" customWidth="1"/>
-    <col min="3" max="3" width="21.8571428571429" customWidth="1"/>
+    <col min="3" max="3" width="25.1428571428571" customWidth="1"/>
     <col min="4" max="4" width="43.1428571428571" customWidth="1"/>
     <col min="5" max="7" width="28.4285714285714" customWidth="1"/>
     <col min="8" max="8" width="37.1428571428571" customWidth="1"/>
@@ -1421,21 +1445,21 @@
         <v>16</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" ht="29" customHeight="1" spans="1:9">
       <c r="A3" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>13</v>
@@ -1444,27 +1468,27 @@
         <v>14</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I3" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" ht="27" spans="1:9">
+      <c r="A4" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="B4" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>13</v>
@@ -1473,71 +1497,71 @@
         <v>14</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" ht="35" customHeight="1" spans="1:9">
       <c r="A5" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="H5" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" ht="27" spans="1:9">
+      <c r="A6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="F6" s="4" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="A6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>14</v>
-      </c>
       <c r="G6" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>22</v>
+        <v>42</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>37</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>18</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
gen api report booking statistic
</commit_message>
<xml_diff>
--- a/src/main/resources/input_excel_file/ApiMaster.xlsx
+++ b/src/main/resources/input_excel_file/ApiMaster.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="50">
   <si>
     <t>module</t>
   </si>
@@ -56,7 +56,7 @@
     <t>test_method_name</t>
   </si>
   <si>
-    <t>login.functional</t>
+    <t>user/functional</t>
   </si>
   <si>
     <t>LoginTest</t>
@@ -74,7 +74,7 @@
     <t>JSON</t>
   </si>
   <si>
-    <t>Login.xlsx</t>
+    <t>user/Login.xlsx</t>
   </si>
   <si>
     <t>login_request_template.json</t>
@@ -83,7 +83,7 @@
     <t>testLogin</t>
   </si>
   <si>
-    <t>booking.functional</t>
+    <t>booking/functional</t>
   </si>
   <si>
     <t>QuoteFeeTest</t>
@@ -95,7 +95,7 @@
     <t>/golf-cms/api/booking/quote-fee</t>
   </si>
   <si>
-    <t>Booking_Quote_Fee.xlsx</t>
+    <t>booking/Booking_Quote_Fee.xlsx</t>
   </si>
   <si>
     <t>quote_fee_request_template.json</t>
@@ -113,7 +113,7 @@
     <t>/golf-cms/api/booking/batch</t>
   </si>
   <si>
-    <t>Create_Booking_Batch.xlsx</t>
+    <t>booking/Create_Booking_Batch.xlsx</t>
   </si>
   <si>
     <t>create_booking_batch_template.json</t>
@@ -137,7 +137,7 @@
     <t>QUERY_PARAM</t>
   </si>
   <si>
-    <t>Get_Booking_List_Select.xlsx</t>
+    <t>booking/Get_Booking_List_Select.xlsx</t>
   </si>
   <si>
     <t>(để trống)</t>
@@ -159,6 +159,24 @@
   </si>
   <si>
     <t>testGetBookingPrice</t>
+  </si>
+  <si>
+    <t>ReportBookingStatisticABC</t>
+  </si>
+  <si>
+    <t>ReportBookingStatisticData</t>
+  </si>
+  <si>
+    <t>/golf-cms/api/report/booking-statistic</t>
+  </si>
+  <si>
+    <t>booking/Report_Booking_Statistic.xlsx</t>
+  </si>
+  <si>
+    <t>report_booking_statistic_template.json</t>
+  </si>
+  <si>
+    <t>testReportBookingStatistic</t>
   </si>
 </sst>
 </file>
@@ -1373,19 +1391,21 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="5"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="6"/>
   <cols>
     <col min="1" max="1" width="24.7142857142857" customWidth="1"/>
     <col min="2" max="2" width="30" customWidth="1"/>
-    <col min="3" max="3" width="25.1428571428571" customWidth="1"/>
-    <col min="4" max="4" width="43.1428571428571" customWidth="1"/>
-    <col min="5" max="7" width="28.4285714285714" customWidth="1"/>
+    <col min="3" max="3" width="26.7142857142857" customWidth="1"/>
+    <col min="4" max="4" width="35.4285714285714" customWidth="1"/>
+    <col min="5" max="5" width="16.2857142857143" customWidth="1"/>
+    <col min="6" max="6" width="19" customWidth="1"/>
+    <col min="7" max="7" width="36.4285714285714" customWidth="1"/>
     <col min="8" max="8" width="37.1428571428571" customWidth="1"/>
     <col min="9" max="9" width="30.4285714285714" customWidth="1"/>
   </cols>
@@ -1564,6 +1584,35 @@
         <v>43</v>
       </c>
     </row>
+    <row r="7" ht="27" spans="1:9">
+      <c r="A7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>